<commit_message>
Create New Text Document.txt
</commit_message>
<xml_diff>
--- a/Work Plan.xlsx
+++ b/Work Plan.xlsx
@@ -4,10 +4,10 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18530" windowHeight="7660"/>
+    <workbookView windowWidth="18468" windowHeight="9215"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Phase 1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
@@ -57,10 +57,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -72,7 +72,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -80,23 +88,15 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -119,21 +119,6 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
       <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -143,6 +128,13 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -163,9 +155,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -181,9 +172,24 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -195,21 +201,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -224,187 +224,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -418,43 +418,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -500,9 +468,41 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -520,148 +520,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="30" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -994,13 +994,13 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="8.73148148148148" defaultRowHeight="14.4" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="32.4545454545455" customWidth="1"/>
-    <col min="2" max="2" width="41.6363636363636" customWidth="1"/>
+    <col min="1" max="1" width="32.4537037037037" customWidth="1"/>
+    <col min="2" max="2" width="41.6388888888889" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1041,7 +1041,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" ht="58" spans="2:2">
+    <row r="8" ht="57.6" spans="2:2">
       <c r="B8" s="1" t="s">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
two terms screen list
</commit_message>
<xml_diff>
--- a/Work Plan.xlsx
+++ b/Work Plan.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18530" windowHeight="6950" activeTab="1"/>
+    <workbookView windowWidth="18530" windowHeight="6950" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="QuaLIS Ver 1.0.0 - Done" sheetId="1" r:id="rId1"/>
     <sheet name="QuaLIS Ver 1.0.1" sheetId="2" r:id="rId2"/>
+    <sheet name="General" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
   <si>
     <t>S. No</t>
   </si>
@@ -135,15 +136,42 @@
   <si>
     <t>Create info file for Setting folder</t>
   </si>
+  <si>
+    <t>Three term screens</t>
+  </si>
+  <si>
+    <t>Unit</t>
+  </si>
+  <si>
+    <t>Storage Condition</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>Designation</t>
+  </si>
+  <si>
+    <t>Division</t>
+  </si>
+  <si>
+    <t>Lab</t>
+  </si>
+  <si>
+    <t>Test Category</t>
+  </si>
+  <si>
+    <t>Product Category</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
@@ -192,13 +220,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -223,27 +244,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -255,6 +259,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -263,45 +275,61 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -334,19 +362,115 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -358,7 +482,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -370,139 +530,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -570,28 +598,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -605,11 +616,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -628,6 +645,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -636,145 +664,145 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="27" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1281,7 +1309,7 @@
   <sheetPr/>
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
@@ -1322,4 +1350,68 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="7" outlineLevelCol="1"/>
+  <cols>
+    <col min="1" max="1" width="18.5454545454545" customWidth="1"/>
+    <col min="2" max="2" width="17.1818181818182" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="2:2">
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2">
+      <c r="B3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2">
+      <c r="B4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2">
+      <c r="B5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2">
+      <c r="B6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2">
+      <c r="B7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2">
+      <c r="B8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>